<commit_message>
Chỉnh sửa CSDL và một số lỗi
</commit_message>
<xml_diff>
--- a/Danh sach thanh vien.xlsx
+++ b/Danh sach thanh vien.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>mntnhan2019@gmail.com</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Nhóm trưởng</t>
+  </si>
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Đường dẫn thùng chứa:http://quanlythuvien5n.googlecode.com/svn/trunk/</t>
+  </si>
+  <si>
+    <t>Đường dẫn đến project: http://code.google.com/p/quanlythuvien5n/</t>
   </si>
 </sst>
 </file>
@@ -70,13 +85,40 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -84,28 +126,6 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="163"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,18 +162,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,22 +471,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -474,7 +495,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,8 +508,11 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -501,8 +525,11 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -515,8 +542,11 @@
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -529,8 +559,11 @@
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -543,8 +576,11 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -556,12 +592,26 @@
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D4" r:id="rId2"/>
@@ -580,8 +630,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -592,8 +643,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>